<commit_message>
adding PIB and Population data to data prep
</commit_message>
<xml_diff>
--- a/data/processed/mnemonico.xlsx
+++ b/data/processed/mnemonico.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rodri\My Git Projects\Spatial-Statistics-Applications\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D052B630-B0B4-4CB8-96C4-00D2E24F931C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE043FCE-CAC6-4BD8-A3C6-214B698F51AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E9A7D7E9-67B1-4E65-B3DA-DC5054B043AF}"/>
+    <workbookView xWindow="2472" yWindow="-9972" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{E9A7D7E9-67B1-4E65-B3DA-DC5054B043AF}"/>
   </bookViews>
   <sheets>
     <sheet name="gas_prices_hist" sheetId="1" r:id="rId1"/>
     <sheet name="gas_prices_station" sheetId="2" r:id="rId2"/>
     <sheet name="PIB" sheetId="3" r:id="rId3"/>
+    <sheet name="Pop" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="187">
   <si>
     <t>index</t>
   </si>
@@ -592,6 +593,27 @@
   </si>
   <si>
     <t>Atividade_3</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>COD. UF</t>
+  </si>
+  <si>
+    <t>COD. MUNIC</t>
+  </si>
+  <si>
+    <t>NOME DO MUNICÍPIO</t>
+  </si>
+  <si>
+    <t>POPULAÇÃO ESTIMADA</t>
+  </si>
+  <si>
+    <t>CdUF</t>
+  </si>
+  <si>
+    <t>PopEstimada</t>
   </si>
 </sst>
 </file>
@@ -1499,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667ABC78-E4D1-4FC1-8D45-B19F88A20009}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,4 +1886,68 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE131B96-88F3-47F7-9A74-AC8625EC76F4}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update PIB and POP
</commit_message>
<xml_diff>
--- a/data/processed/mnemonico.xlsx
+++ b/data/processed/mnemonico.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rodri\My Git Projects\Spatial-Statistics-Applications\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rodri\My GIT Projects\Spatial-Statistics-Applications\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE043FCE-CAC6-4BD8-A3C6-214B698F51AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED84568-B216-4090-BA1A-7ECDAA396EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2472" yWindow="-9972" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{E9A7D7E9-67B1-4E65-B3DA-DC5054B043AF}"/>
+    <workbookView xWindow="2124" yWindow="-10320" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{E9A7D7E9-67B1-4E65-B3DA-DC5054B043AF}"/>
   </bookViews>
   <sheets>
     <sheet name="gas_prices_hist" sheetId="1" r:id="rId1"/>
     <sheet name="gas_prices_station" sheetId="2" r:id="rId2"/>
     <sheet name="PIB" sheetId="3" r:id="rId3"/>
     <sheet name="Pop" sheetId="4" r:id="rId4"/>
+    <sheet name="PIB_change" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="201">
   <si>
     <t>index</t>
   </si>
@@ -614,6 +615,48 @@
   </si>
   <si>
     <t>PopEstimada</t>
+  </si>
+  <si>
+    <t>PIB_2016</t>
+  </si>
+  <si>
+    <t>PIB_2017</t>
+  </si>
+  <si>
+    <t>PIBCap2016</t>
+  </si>
+  <si>
+    <t>PIBCap2017</t>
+  </si>
+  <si>
+    <t>ChgPIB</t>
+  </si>
+  <si>
+    <t>ChgPIBCap</t>
+  </si>
+  <si>
+    <t>PopEst</t>
+  </si>
+  <si>
+    <t>PIB a preços correntes de 2016</t>
+  </si>
+  <si>
+    <t>PIB a preços correntes de 2017</t>
+  </si>
+  <si>
+    <t>PIB per capta a preços correntes de 2016</t>
+  </si>
+  <si>
+    <t>PIB per capta a preços correntes de 2017</t>
+  </si>
+  <si>
+    <t>Variação do PIB de 2017 para 2016</t>
+  </si>
+  <si>
+    <t>Variação do PIB per Capta de 2017 para 2016</t>
+  </si>
+  <si>
+    <t>Populção Estimada</t>
   </si>
 </sst>
 </file>
@@ -968,7 +1011,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1892,7 +1935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE131B96-88F3-47F7-9A74-AC8625EC76F4}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1950,4 +1995,94 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442441A6-3218-4EB7-8345-9AFD7F53D12E}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding x and y coordinates on munip shapefile
</commit_message>
<xml_diff>
--- a/data/processed/mnemonico.xlsx
+++ b/data/processed/mnemonico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rodri\My GIT Projects\Spatial-Statistics-Applications\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D942E85-5054-4F0C-AD4C-D8D6C8D937D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97D4B84-C868-4493-BF0E-A553186C409E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2124" yWindow="-10320" windowWidth="17280" windowHeight="8964" xr2:uid="{E9A7D7E9-67B1-4E65-B3DA-DC5054B043AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E9A7D7E9-67B1-4E65-B3DA-DC5054B043AF}"/>
   </bookViews>
   <sheets>
     <sheet name="gas_prices_hist" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="204">
   <si>
     <t>index</t>
   </si>
@@ -654,6 +654,18 @@
   </si>
   <si>
     <t>Populção Estimada</t>
+  </si>
+  <si>
+    <t>X_COORD</t>
+  </si>
+  <si>
+    <t>Y_COORD</t>
+  </si>
+  <si>
+    <t>X cordenada da sede do município</t>
+  </si>
+  <si>
+    <t>Y cordenada da sede do município</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC38ADB-3BE1-4C49-A6B5-3A77CABD8E46}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1346,6 +1358,22 @@
       </c>
       <c r="B41" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>